<commit_message>
Removed all js > 1000
</commit_message>
<xml_diff>
--- a/results/javascript/create-react-app/create-react-app.xlsx
+++ b/results/javascript/create-react-app/create-react-app.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamc\Desktop\results\javascript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamc\Documents\CodeSize\CodeSize\results\javascript\create-react-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6834B6F3-C7C7-4B21-9992-7894FA0FC803}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D45DC8-1C5C-4F69-91DB-A653A3520245}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="create-react-app2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="303">
   <si>
     <t>File</t>
   </si>
@@ -934,7 +942,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1770,11 +1778,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O252"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,24 +1845,24 @@
         <v>299</v>
       </c>
       <c r="K2" s="2">
-        <f>MAX(C2:C252)</f>
+        <f>MAX(C2:C251)</f>
         <v>660</v>
       </c>
       <c r="L2" s="2">
-        <f>MIN(C2:C252)</f>
+        <f>MIN(C2:C251)</f>
         <v>1</v>
       </c>
       <c r="M2" s="2">
-        <f>AVERAGE(C2:C252)</f>
-        <v>47.717131474103589</v>
+        <f>AVERAGE(C2:C251)</f>
+        <v>46.356000000000002</v>
       </c>
       <c r="N2" s="2">
-        <f>_xlfn.STDEV.P(C2:C252)</f>
-        <v>72.6073025514888</v>
+        <f>_xlfn.STDEV.P(C2:C251)</f>
+        <v>69.482985428088796</v>
       </c>
       <c r="O2" s="2">
-        <f>N2/SQRT(COUNT(C2:C252))</f>
-        <v>4.5829322994528576</v>
+        <f>N2/SQRT(COUNT(C2:C251))</f>
+        <v>4.3944898516210049</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1880,24 +1888,24 @@
         <v>300</v>
       </c>
       <c r="K3" s="2">
-        <f>MAX(D2:D252)</f>
-        <v>7287</v>
+        <f>MAX(D2:D251)</f>
+        <v>232</v>
       </c>
       <c r="L3" s="2">
-        <f>MIN(D2:D252)</f>
+        <f>MIN(D2:D251)</f>
         <v>17</v>
       </c>
       <c r="M3" s="2">
-        <f>AVERAGE(D2:D252)</f>
-        <v>107.2191235059761</v>
+        <f>AVERAGE(D2:D251)</f>
+        <v>78.5</v>
       </c>
       <c r="N3" s="2">
-        <f>_xlfn.STDEV.P(D2:D252)</f>
-        <v>456.09914063553634</v>
+        <f>_xlfn.STDEV.P(D2:D251)</f>
+        <v>42.85708809520311</v>
       </c>
       <c r="O3" s="2">
-        <f>N3/SQRT(COUNT(D2:D252))</f>
-        <v>28.788722482686836</v>
+        <f>N3/SQRT(COUNT(D2:D251))</f>
+        <v>2.7105202452665802</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1923,24 +1931,24 @@
         <v>301</v>
       </c>
       <c r="K4" s="2">
-        <f>MAX(E2:E252)</f>
+        <f>MAX(E2:E251)</f>
         <v>14</v>
       </c>
       <c r="L4" s="2">
-        <f>MIN(E2:E252)</f>
+        <f>MIN(E2:E251)</f>
         <v>0</v>
       </c>
       <c r="M4" s="2">
-        <f>AVERAGE(E2:E252)</f>
-        <v>4.5577689243027892</v>
+        <f>AVERAGE(E2:E251)</f>
+        <v>4.5759999999999996</v>
       </c>
       <c r="N4" s="2">
-        <f>_xlfn.STDEV.P(E2:E252)</f>
-        <v>3.3075504293991296</v>
+        <f>_xlfn.STDEV.P(E2:E251)</f>
+        <v>3.3015487274913875</v>
       </c>
       <c r="O4" s="2">
-        <f>N4/SQRT(COUNT(E2:E252))</f>
-        <v>0.20877073190004661</v>
+        <f>N4/SQRT(COUNT(E2:E251))</f>
+        <v>0.20880827569806712</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1966,23 +1974,23 @@
         <v>302</v>
       </c>
       <c r="K5" s="2">
-        <f>MAX(F2:F252)</f>
+        <f>MAX(F2:F251)</f>
         <v>0</v>
       </c>
       <c r="L5" s="2">
-        <f>MIN(F2:F252)</f>
+        <f>MIN(F2:F251)</f>
         <v>0</v>
       </c>
       <c r="M5" s="2">
-        <f>AVERAGE(F2:F252)</f>
+        <f>AVERAGE(F2:F251)</f>
         <v>0</v>
       </c>
       <c r="N5" s="2">
-        <f>_xlfn.STDEV.P(F2:F252)</f>
+        <f>_xlfn.STDEV.P(F2:F251)</f>
         <v>0</v>
       </c>
       <c r="O5" s="2">
-        <f>N5/SQRT(COUNT(F2:F252))</f>
+        <f>N5/SQRT(COUNT(F2:F251))</f>
         <v>0</v>
       </c>
     </row>
@@ -4788,19 +4796,19 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B146" t="s">
+        <v>187</v>
+      </c>
+      <c r="C146">
         <v>7</v>
       </c>
-      <c r="C146">
-        <v>388</v>
-      </c>
       <c r="D146">
-        <v>7287</v>
+        <v>52</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F146">
         <v>0</v>
@@ -4811,16 +4819,16 @@
         <v>186</v>
       </c>
       <c r="B147" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C147">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="D147">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="E147">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F147">
         <v>0</v>
@@ -4831,16 +4839,16 @@
         <v>186</v>
       </c>
       <c r="B148" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C148">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="D148">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E148">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F148">
         <v>0</v>
@@ -4851,16 +4859,16 @@
         <v>186</v>
       </c>
       <c r="B149" t="s">
-        <v>189</v>
+        <v>7</v>
       </c>
       <c r="C149">
-        <v>25</v>
+        <v>157</v>
       </c>
       <c r="D149">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E149">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F149">
         <v>0</v>
@@ -4871,16 +4879,16 @@
         <v>186</v>
       </c>
       <c r="B150" t="s">
-        <v>7</v>
+        <v>190</v>
       </c>
       <c r="C150">
-        <v>157</v>
+        <v>19</v>
       </c>
       <c r="D150">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E150">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F150">
         <v>0</v>
@@ -4891,16 +4899,16 @@
         <v>186</v>
       </c>
       <c r="B151" t="s">
-        <v>190</v>
+        <v>7</v>
       </c>
       <c r="C151">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="D151">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E151">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F151">
         <v>0</v>
@@ -4908,19 +4916,19 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B152" t="s">
-        <v>7</v>
+        <v>192</v>
       </c>
       <c r="C152">
-        <v>157</v>
+        <v>34</v>
       </c>
       <c r="D152">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E152">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F152">
         <v>0</v>
@@ -4928,19 +4936,19 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B153" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C153">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D153">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E153">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F153">
         <v>0</v>
@@ -4951,16 +4959,16 @@
         <v>193</v>
       </c>
       <c r="B154" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C154">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="D154">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="E154">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F154">
         <v>0</v>
@@ -4971,16 +4979,16 @@
         <v>193</v>
       </c>
       <c r="B155" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C155">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="D155">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="E155">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F155">
         <v>0</v>
@@ -4991,16 +4999,16 @@
         <v>193</v>
       </c>
       <c r="B156" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C156">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="D156">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E156">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F156">
         <v>0</v>
@@ -5011,16 +5019,16 @@
         <v>193</v>
       </c>
       <c r="B157" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C157">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D157">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="E157">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F157">
         <v>0</v>
@@ -5031,16 +5039,16 @@
         <v>193</v>
       </c>
       <c r="B158" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C158">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D158">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E158">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F158">
         <v>0</v>
@@ -5051,16 +5059,16 @@
         <v>193</v>
       </c>
       <c r="B159" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C159">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D159">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E159">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F159">
         <v>0</v>
@@ -5071,16 +5079,16 @@
         <v>193</v>
       </c>
       <c r="B160" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C160">
+        <v>77</v>
+      </c>
+      <c r="D160">
+        <v>98</v>
+      </c>
+      <c r="E160">
         <v>8</v>
-      </c>
-      <c r="D160">
-        <v>60</v>
-      </c>
-      <c r="E160">
-        <v>12</v>
       </c>
       <c r="F160">
         <v>0</v>
@@ -5091,16 +5099,16 @@
         <v>193</v>
       </c>
       <c r="B161" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C161">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="D161">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E161">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F161">
         <v>0</v>
@@ -5108,19 +5116,19 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B162" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C162">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="D162">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="E162">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F162">
         <v>0</v>
@@ -5128,19 +5136,19 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B163" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C163">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D163">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E163">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F163">
         <v>0</v>
@@ -5148,19 +5156,19 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B164" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C164">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D164">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E164">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F164">
         <v>0</v>
@@ -5168,16 +5176,16 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B165" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C165">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D165">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="E165">
         <v>2</v>
@@ -5188,19 +5196,19 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B166" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C166">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D166">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="E166">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F166">
         <v>0</v>
@@ -5211,16 +5219,16 @@
         <v>211</v>
       </c>
       <c r="B167" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C167">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D167">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="E167">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F167">
         <v>0</v>
@@ -5231,13 +5239,13 @@
         <v>211</v>
       </c>
       <c r="B168" t="s">
-        <v>213</v>
+        <v>58</v>
       </c>
       <c r="C168">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D168">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="E168">
         <v>4</v>
@@ -5251,16 +5259,16 @@
         <v>211</v>
       </c>
       <c r="B169" t="s">
-        <v>58</v>
+        <v>214</v>
       </c>
       <c r="C169">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D169">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="E169">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F169">
         <v>0</v>
@@ -5271,16 +5279,16 @@
         <v>211</v>
       </c>
       <c r="B170" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C170">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D170">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E170">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F170">
         <v>0</v>
@@ -5291,16 +5299,16 @@
         <v>211</v>
       </c>
       <c r="B171" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C171">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D171">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="E171">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F171">
         <v>0</v>
@@ -5311,10 +5319,10 @@
         <v>211</v>
       </c>
       <c r="B172" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C172">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D172">
         <v>61</v>
@@ -5331,16 +5339,16 @@
         <v>211</v>
       </c>
       <c r="B173" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C173">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D173">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E173">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F173">
         <v>0</v>
@@ -5351,16 +5359,16 @@
         <v>211</v>
       </c>
       <c r="B174" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C174">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D174">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="E174">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F174">
         <v>0</v>
@@ -5371,16 +5379,16 @@
         <v>211</v>
       </c>
       <c r="B175" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C175">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D175">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="E175">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F175">
         <v>0</v>
@@ -5391,16 +5399,16 @@
         <v>211</v>
       </c>
       <c r="B176" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C176">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D176">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E176">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F176">
         <v>0</v>
@@ -5411,13 +5419,13 @@
         <v>211</v>
       </c>
       <c r="B177" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C177">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D177">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="E177">
         <v>2</v>
@@ -5431,16 +5439,16 @@
         <v>211</v>
       </c>
       <c r="B178" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C178">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D178">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E178">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F178">
         <v>0</v>
@@ -5451,16 +5459,16 @@
         <v>211</v>
       </c>
       <c r="B179" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C179">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D179">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E179">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F179">
         <v>0</v>
@@ -5471,13 +5479,13 @@
         <v>211</v>
       </c>
       <c r="B180" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C180">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D180">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="E180">
         <v>2</v>
@@ -5491,16 +5499,16 @@
         <v>211</v>
       </c>
       <c r="B181" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C181">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D181">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="E181">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F181">
         <v>0</v>
@@ -5511,16 +5519,16 @@
         <v>211</v>
       </c>
       <c r="B182" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C182">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D182">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="E182">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F182">
         <v>0</v>
@@ -5531,13 +5539,13 @@
         <v>211</v>
       </c>
       <c r="B183" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C183">
         <v>3</v>
       </c>
       <c r="D183">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E183">
         <v>8</v>
@@ -5551,16 +5559,16 @@
         <v>211</v>
       </c>
       <c r="B184" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C184">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D184">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="E184">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F184">
         <v>0</v>
@@ -5568,16 +5576,16 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="B185" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C185">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D185">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E185">
         <v>2</v>
@@ -5591,13 +5599,13 @@
         <v>230</v>
       </c>
       <c r="B186" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C186">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D186">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E186">
         <v>2</v>
@@ -5611,13 +5619,13 @@
         <v>230</v>
       </c>
       <c r="B187" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C187">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D187">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E187">
         <v>2</v>
@@ -5631,16 +5639,16 @@
         <v>230</v>
       </c>
       <c r="B188" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C188">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D188">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E188">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F188">
         <v>0</v>
@@ -5651,16 +5659,16 @@
         <v>230</v>
       </c>
       <c r="B189" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C189">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D189">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E189">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F189">
         <v>0</v>
@@ -5671,16 +5679,16 @@
         <v>230</v>
       </c>
       <c r="B190" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C190">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D190">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E190">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F190">
         <v>0</v>
@@ -5688,16 +5696,16 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="B191" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C191">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D191">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="E191">
         <v>4</v>
@@ -5711,16 +5719,16 @@
         <v>237</v>
       </c>
       <c r="B192" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C192">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D192">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E192">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F192">
         <v>0</v>
@@ -5731,16 +5739,16 @@
         <v>237</v>
       </c>
       <c r="B193" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C193">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D193">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="E193">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F193">
         <v>0</v>
@@ -5748,19 +5756,19 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B194" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C194">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D194">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="E194">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F194">
         <v>0</v>
@@ -5771,16 +5779,16 @@
         <v>241</v>
       </c>
       <c r="B195" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C195">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D195">
         <v>77</v>
       </c>
       <c r="E195">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F195">
         <v>0</v>
@@ -5788,19 +5796,19 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B196" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C196">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D196">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E196">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F196">
         <v>0</v>
@@ -5811,16 +5819,16 @@
         <v>244</v>
       </c>
       <c r="B197" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C197">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="D197">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="E197">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F197">
         <v>0</v>
@@ -5831,16 +5839,16 @@
         <v>244</v>
       </c>
       <c r="B198" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C198">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="D198">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="E198">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F198">
         <v>0</v>
@@ -5857,7 +5865,7 @@
         <v>3</v>
       </c>
       <c r="D199">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E199">
         <v>2</v>
@@ -5871,13 +5879,13 @@
         <v>244</v>
       </c>
       <c r="B200" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C200">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D200">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="E200">
         <v>2</v>
@@ -5888,19 +5896,19 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B201" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C201">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D201">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E201">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F201">
         <v>0</v>
@@ -5908,19 +5916,19 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B202" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C202">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D202">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="E202">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F202">
         <v>0</v>
@@ -5928,16 +5936,16 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B203" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C203">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D203">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E203">
         <v>2</v>
@@ -5951,16 +5959,16 @@
         <v>253</v>
       </c>
       <c r="B204" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C204">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D204">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E204">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F204">
         <v>0</v>
@@ -5971,16 +5979,16 @@
         <v>253</v>
       </c>
       <c r="B205" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C205">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D205">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="E205">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F205">
         <v>0</v>
@@ -5991,16 +5999,16 @@
         <v>253</v>
       </c>
       <c r="B206" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C206">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D206">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="E206">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F206">
         <v>0</v>
@@ -6008,16 +6016,16 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B207" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C207">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D207">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E207">
         <v>6</v>
@@ -6031,10 +6039,10 @@
         <v>258</v>
       </c>
       <c r="B208" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C208">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D208">
         <v>66</v>
@@ -6048,19 +6056,19 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B209" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C209">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D209">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E209">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F209">
         <v>0</v>
@@ -6071,13 +6079,13 @@
         <v>261</v>
       </c>
       <c r="B210" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C210">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D210">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E210">
         <v>2</v>
@@ -6091,16 +6099,16 @@
         <v>261</v>
       </c>
       <c r="B211" t="s">
-        <v>263</v>
+        <v>7</v>
       </c>
       <c r="C211">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D211">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E211">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F211">
         <v>0</v>
@@ -6108,19 +6116,19 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B212" t="s">
-        <v>7</v>
+        <v>265</v>
       </c>
       <c r="C212">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="D212">
-        <v>78</v>
+        <v>151</v>
       </c>
       <c r="E212">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F212">
         <v>0</v>
@@ -6128,13 +6136,13 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B213" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C213">
-        <v>109</v>
+        <v>178</v>
       </c>
       <c r="D213">
         <v>151</v>
@@ -6148,19 +6156,19 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B214" t="s">
-        <v>267</v>
+        <v>47</v>
       </c>
       <c r="C214">
-        <v>178</v>
+        <v>21</v>
       </c>
       <c r="D214">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="E214">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F214">
         <v>0</v>
@@ -6168,19 +6176,19 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B215" t="s">
-        <v>47</v>
+        <v>265</v>
       </c>
       <c r="C215">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D215">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E215">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F215">
         <v>0</v>
@@ -6188,16 +6196,16 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B216" t="s">
         <v>265</v>
       </c>
       <c r="C216">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D216">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E216">
         <v>2</v>
@@ -6208,7 +6216,7 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B217" t="s">
         <v>265</v>
@@ -6217,7 +6225,7 @@
         <v>3</v>
       </c>
       <c r="D217">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E217">
         <v>2</v>
@@ -6228,7 +6236,7 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B218" t="s">
         <v>265</v>
@@ -6237,7 +6245,7 @@
         <v>3</v>
       </c>
       <c r="D218">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E218">
         <v>2</v>
@@ -6248,19 +6256,19 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B219" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C219">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D219">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="E219">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F219">
         <v>0</v>
@@ -6271,13 +6279,13 @@
         <v>273</v>
       </c>
       <c r="B220" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C220">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="D220">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="E220">
         <v>6</v>
@@ -6291,16 +6299,16 @@
         <v>273</v>
       </c>
       <c r="B221" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C221">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="D221">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="E221">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F221">
         <v>0</v>
@@ -6311,16 +6319,16 @@
         <v>273</v>
       </c>
       <c r="B222" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C222">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="D222">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="E222">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F222">
         <v>0</v>
@@ -6331,16 +6339,16 @@
         <v>273</v>
       </c>
       <c r="B223" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C223">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D223">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="E223">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F223">
         <v>0</v>
@@ -6351,16 +6359,16 @@
         <v>273</v>
       </c>
       <c r="B224" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C224">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D224">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="E224">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F224">
         <v>0</v>
@@ -6371,16 +6379,16 @@
         <v>273</v>
       </c>
       <c r="B225" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C225">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D225">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="E225">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F225">
         <v>0</v>
@@ -6391,13 +6399,13 @@
         <v>273</v>
       </c>
       <c r="B226" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C226">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D226">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="E226">
         <v>4</v>
@@ -6411,16 +6419,16 @@
         <v>273</v>
       </c>
       <c r="B227" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C227">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D227">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E227">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F227">
         <v>0</v>
@@ -6431,16 +6439,16 @@
         <v>273</v>
       </c>
       <c r="B228" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C228">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D228">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E228">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F228">
         <v>0</v>
@@ -6451,16 +6459,16 @@
         <v>273</v>
       </c>
       <c r="B229" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C229">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D229">
         <v>79</v>
       </c>
       <c r="E229">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F229">
         <v>0</v>
@@ -6471,16 +6479,16 @@
         <v>273</v>
       </c>
       <c r="B230" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C230">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D230">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E230">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F230">
         <v>0</v>
@@ -6491,16 +6499,16 @@
         <v>273</v>
       </c>
       <c r="B231" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C231">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D231">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E231">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F231">
         <v>0</v>
@@ -6511,13 +6519,13 @@
         <v>273</v>
       </c>
       <c r="B232" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C232">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="D232">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="E232">
         <v>6</v>
@@ -6531,16 +6539,16 @@
         <v>273</v>
       </c>
       <c r="B233" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C233">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="D233">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="E233">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F233">
         <v>0</v>
@@ -6551,16 +6559,16 @@
         <v>273</v>
       </c>
       <c r="B234" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C234">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D234">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="E234">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F234">
         <v>0</v>
@@ -6571,16 +6579,16 @@
         <v>273</v>
       </c>
       <c r="B235" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C235">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D235">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E235">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F235">
         <v>0</v>
@@ -6588,19 +6596,19 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
       <c r="B236" t="s">
-        <v>290</v>
+        <v>7</v>
       </c>
       <c r="C236">
-        <v>19</v>
+        <v>188</v>
       </c>
       <c r="D236">
-        <v>59</v>
+        <v>232</v>
       </c>
       <c r="E236">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F236">
         <v>0</v>
@@ -6611,16 +6619,16 @@
         <v>291</v>
       </c>
       <c r="B237" t="s">
-        <v>7</v>
+        <v>292</v>
       </c>
       <c r="C237">
-        <v>188</v>
+        <v>3</v>
       </c>
       <c r="D237">
-        <v>232</v>
+        <v>78</v>
       </c>
       <c r="E237">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F237">
         <v>0</v>
@@ -6631,16 +6639,16 @@
         <v>291</v>
       </c>
       <c r="B238" t="s">
-        <v>292</v>
+        <v>7</v>
       </c>
       <c r="C238">
-        <v>3</v>
+        <v>188</v>
       </c>
       <c r="D238">
-        <v>78</v>
+        <v>232</v>
       </c>
       <c r="E238">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F238">
         <v>0</v>
@@ -6888,41 +6896,21 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B251" t="s">
         <v>7</v>
       </c>
       <c r="C251">
-        <v>188</v>
+        <v>117</v>
       </c>
       <c r="D251">
-        <v>232</v>
+        <v>83</v>
       </c>
       <c r="E251">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F251">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>293</v>
-      </c>
-      <c r="B252" t="s">
-        <v>7</v>
-      </c>
-      <c r="C252">
-        <v>117</v>
-      </c>
-      <c r="D252">
-        <v>83</v>
-      </c>
-      <c r="E252">
-        <v>4</v>
-      </c>
-      <c r="F252">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
javscript stdev.p -> stdev.s
</commit_message>
<xml_diff>
--- a/results/javascript/create-react-app/create-react-app.xlsx
+++ b/results/javascript/create-react-app/create-react-app.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamc\Documents\CodeSize\CodeSize\results\javascript\create-react-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashort11/research/CodeSize/results/javascript/create-react-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D45DC8-1C5C-4F69-91DB-A653A3520245}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4401250A-94DD-164A-9C1E-DB3EEF8E7735}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="create-react-app2" sheetId="1" r:id="rId1"/>
@@ -1782,12 +1782,12 @@
   <dimension ref="A1:O251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1857,15 +1857,15 @@
         <v>46.356000000000002</v>
       </c>
       <c r="N2" s="2">
-        <f>_xlfn.STDEV.P(C2:C251)</f>
-        <v>69.482985428088796</v>
+        <f>_xlfn.STDEV.S(C2:C251)</f>
+        <v>69.622369691398632</v>
       </c>
       <c r="O2" s="2">
         <f>N2/SQRT(COUNT(C2:C251))</f>
-        <v>4.3944898516210049</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4.4033052864618796</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1900,15 +1900,15 @@
         <v>78.5</v>
       </c>
       <c r="N3" s="2">
-        <f>_xlfn.STDEV.P(D2:D251)</f>
-        <v>42.85708809520311</v>
+        <f>_xlfn.STDEV.S(D2:D251)</f>
+        <v>42.943060274074682</v>
       </c>
       <c r="O3" s="2">
         <f>N3/SQRT(COUNT(D2:D251))</f>
-        <v>2.7105202452665802</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2.7159576032794113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1943,15 +1943,15 @@
         <v>4.5759999999999996</v>
       </c>
       <c r="N4" s="2">
-        <f>_xlfn.STDEV.P(E2:E251)</f>
-        <v>3.3015487274913875</v>
+        <f>_xlfn.STDEV.S(E2:E251)</f>
+        <v>3.3081717005016529</v>
       </c>
       <c r="O4" s="2">
         <f>N4/SQRT(COUNT(E2:E251))</f>
-        <v>0.20880827569806712</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.20922714928995231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="2">
-        <f>_xlfn.STDEV.P(F2:F251)</f>
+        <f>_xlfn.STDEV.S(F2:F251)</f>
         <v>0</v>
       </c>
       <c r="O5" s="2">
@@ -1994,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>71</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>78</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>84</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>84</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>88</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>92</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>92</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>95</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>95</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>95</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>95</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>95</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>95</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>110</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>114</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>116</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>118</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>120</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>122</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>124</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>126</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>128</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>130</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>130</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>133</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>133</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>136</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>136</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>136</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>140</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>140</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>143</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>145</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>147</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>147</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>150</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>150</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>150</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>150</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>155</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>155</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>158</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>158</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>158</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>162</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>162</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>162</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>166</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>166</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>166</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>169</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>169</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>170</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>170</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>170</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>173</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>174</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>176</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>176</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>179</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>179</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>182</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>182</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>182</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>186</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>186</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>186</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>186</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>186</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>186</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>191</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>193</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>193</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>193</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>193</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>193</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>193</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>193</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>193</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>193</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>203</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>205</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>207</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>209</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>211</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>211</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>211</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>211</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>211</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>211</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>211</v>
       </c>
@@ -5334,7 +5334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>211</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>211</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>211</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>211</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>211</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>211</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>211</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>211</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>211</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>211</v>
       </c>
@@ -5534,7 +5534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>211</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>211</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>230</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>230</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>230</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>230</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>230</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>230</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>237</v>
       </c>
@@ -5714,7 +5714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>237</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>237</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>241</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>241</v>
       </c>
@@ -5794,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>244</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>244</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>244</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>244</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>244</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>249</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>251</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>253</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>253</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>253</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>253</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>258</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>258</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>261</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>261</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>261</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>264</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>266</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>268</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>269</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>270</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>271</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>272</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>273</v>
       </c>
@@ -6274,7 +6274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>273</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>273</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>273</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>273</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>273</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>273</v>
       </c>
@@ -6394,7 +6394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>273</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>273</v>
       </c>
@@ -6434,7 +6434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>273</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>273</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>273</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>273</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>273</v>
       </c>
@@ -6534,7 +6534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>273</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>273</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>273</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>291</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>291</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>291</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>291</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>291</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>291</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>291</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>291</v>
       </c>
@@ -6754,7 +6754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>291</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>291</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>291</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>291</v>
       </c>
@@ -6834,7 +6834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>291</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>291</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>291</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>293</v>
       </c>

</xml_diff>